<commit_message>
Fixed up the Excel workbooks for each of the countires and updated the corresponding .txt files as well.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/IranDataWorkbook.xlsx
+++ b/data/Excel Workbooks/IranDataWorkbook.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="21075" windowHeight="9795"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="21075" windowHeight="9795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Iran Workbook" sheetId="1" r:id="rId1"/>
-    <sheet name="Iran Indices Comparison" sheetId="7" r:id="rId2"/>
-    <sheet name="Employment calcs" sheetId="2" r:id="rId3"/>
-    <sheet name="Exergy calcs" sheetId="8" r:id="rId4"/>
+    <sheet name="IRData" sheetId="9" r:id="rId2"/>
+    <sheet name="Iran Indices Comparison" sheetId="7" r:id="rId3"/>
+    <sheet name="Employment calcs" sheetId="2" r:id="rId4"/>
+    <sheet name="Exergy calcs" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
   <si>
     <t>Notes</t>
   </si>
@@ -806,17 +807,39 @@
   <si>
     <t>Employment [Persons ages 15+]</t>
   </si>
+  <si>
+    <t xml:space="preserve"> - The 'IRData' tab has the indexed data from this page formatted for direct exporting into R (a statistical analysis program).</t>
+  </si>
+  <si>
+    <t>iYear</t>
+  </si>
+  <si>
+    <t>iGDP</t>
+  </si>
+  <si>
+    <t>iLabor</t>
+  </si>
+  <si>
+    <t>iCapStk</t>
+  </si>
+  <si>
+    <t>iQ</t>
+  </si>
+  <si>
+    <t>iX</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="172" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="38">
     <font>
@@ -2176,7 +2199,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2357,14 +2380,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2377,16 +2399,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2395,11 +2417,20 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="481">
@@ -2969,7 +3000,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$A$10:$A$30</c:f>
+              <c:f>'Iran Workbook'!$A$12:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3041,7 +3072,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$G$10:$G$30</c:f>
+              <c:f>'Iran Workbook'!$H$12:$H$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3133,7 +3164,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$A$10:$A$30</c:f>
+              <c:f>'Iran Workbook'!$A$12:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3205,7 +3236,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$I$10:$I$30</c:f>
+              <c:f>'Iran Workbook'!$J$12:$J$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3295,7 +3326,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$A$10:$A$30</c:f>
+              <c:f>'Iran Workbook'!$A$12:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3367,7 +3398,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$H$10:$H$30</c:f>
+              <c:f>'Iran Workbook'!$I$12:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3459,7 +3490,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$A$10:$A$30</c:f>
+              <c:f>'Iran Workbook'!$A$12:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3531,7 +3562,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$K$10:$K$30</c:f>
+              <c:f>'Iran Workbook'!$L$12:$L$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3625,7 +3656,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$A$10:$A$30</c:f>
+              <c:f>'Iran Workbook'!$A$12:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3697,7 +3728,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Iran Workbook'!$J$10:$J$30</c:f>
+              <c:f>'Iran Workbook'!$K$12:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
@@ -3777,11 +3808,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113388160"/>
-        <c:axId val="193584128"/>
+        <c:axId val="78765440"/>
+        <c:axId val="96008064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113388160"/>
+        <c:axId val="78765440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3814,12 +3845,12 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193584128"/>
+        <c:crossAx val="96008064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="193584128"/>
+        <c:axId val="96008064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -3853,7 +3884,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113388160"/>
+        <c:crossAx val="78765440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -4535,10 +4566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC33"/>
+  <dimension ref="A1:BD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4548,25 +4579,27 @@
     <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" style="75" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" style="81" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="79" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" style="79" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="12" customFormat="1">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:56" s="12" customFormat="1">
+      <c r="A1" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
       <c r="E1" s="77"/>
-      <c r="J1" s="81"/>
-    </row>
-    <row r="2" spans="1:55">
+      <c r="G1" s="79"/>
+      <c r="K1" s="79"/>
+    </row>
+    <row r="2" spans="1:56">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -4576,12 +4609,12 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:55">
+      <c r="J2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:56">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>36</v>
@@ -4589,12 +4622,12 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:55">
+      <c r="J3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:56">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>96</v>
@@ -4602,12 +4635,12 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:55">
+      <c r="J4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:56">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>37</v>
@@ -4615,12 +4648,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:55">
+      <c r="J5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:56">
       <c r="A6" s="6"/>
       <c r="B6" s="74" t="s">
         <v>91</v>
@@ -4629,11 +4662,11 @@
       <c r="D6" s="9"/>
       <c r="E6" s="76"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="76"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="76"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -4676,125 +4709,175 @@
       <c r="AY6" s="9"/>
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
-      <c r="BB6" s="6"/>
+      <c r="BB6" s="9"/>
       <c r="BC6" s="6"/>
-    </row>
-    <row r="8" spans="1:55" ht="15" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="82" t="s">
+      <c r="BD6" s="6"/>
+    </row>
+    <row r="7" spans="1:56" s="79" customFormat="1">
+      <c r="B7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="76"/>
+      <c r="R7" s="76"/>
+      <c r="S7" s="76"/>
+      <c r="T7" s="76"/>
+      <c r="U7" s="76"/>
+      <c r="V7" s="76"/>
+      <c r="W7" s="76"/>
+      <c r="X7" s="76"/>
+      <c r="Y7" s="76"/>
+      <c r="Z7" s="76"/>
+      <c r="AA7" s="76"/>
+      <c r="AB7" s="76"/>
+      <c r="AC7" s="76"/>
+      <c r="AD7" s="76"/>
+      <c r="AE7" s="76"/>
+      <c r="AF7" s="76"/>
+      <c r="AG7" s="76"/>
+      <c r="AH7" s="76"/>
+      <c r="AI7" s="76"/>
+      <c r="AJ7" s="76"/>
+      <c r="AK7" s="76"/>
+      <c r="AL7" s="76"/>
+      <c r="AM7" s="76"/>
+      <c r="AN7" s="76"/>
+      <c r="AO7" s="76"/>
+      <c r="AP7" s="76"/>
+      <c r="AQ7" s="76"/>
+      <c r="AR7" s="76"/>
+      <c r="AS7" s="76"/>
+      <c r="AT7" s="76"/>
+      <c r="AU7" s="76"/>
+      <c r="AV7" s="76"/>
+      <c r="AW7" s="76"/>
+      <c r="AX7" s="76"/>
+      <c r="AY7" s="76"/>
+      <c r="AZ7" s="76"/>
+      <c r="BA7" s="76"/>
+      <c r="BB7" s="76"/>
+    </row>
+    <row r="8" spans="1:56" s="79" customFormat="1">
+      <c r="B8" s="76"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="76"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="76"/>
+      <c r="U8" s="76"/>
+      <c r="V8" s="76"/>
+      <c r="W8" s="76"/>
+      <c r="X8" s="76"/>
+      <c r="Y8" s="76"/>
+      <c r="Z8" s="76"/>
+      <c r="AA8" s="76"/>
+      <c r="AB8" s="76"/>
+      <c r="AC8" s="76"/>
+      <c r="AD8" s="76"/>
+      <c r="AE8" s="76"/>
+      <c r="AF8" s="76"/>
+      <c r="AG8" s="76"/>
+      <c r="AH8" s="76"/>
+      <c r="AI8" s="76"/>
+      <c r="AJ8" s="76"/>
+      <c r="AK8" s="76"/>
+      <c r="AL8" s="76"/>
+      <c r="AM8" s="76"/>
+      <c r="AN8" s="76"/>
+      <c r="AO8" s="76"/>
+      <c r="AP8" s="76"/>
+      <c r="AQ8" s="76"/>
+      <c r="AR8" s="76"/>
+      <c r="AS8" s="76"/>
+      <c r="AT8" s="76"/>
+      <c r="AU8" s="76"/>
+      <c r="AV8" s="76"/>
+      <c r="AW8" s="76"/>
+      <c r="AX8" s="76"/>
+      <c r="AY8" s="76"/>
+      <c r="AZ8" s="76"/>
+      <c r="BA8" s="76"/>
+      <c r="BB8" s="76"/>
+    </row>
+    <row r="9" spans="1:56">
+      <c r="G9" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" ht="15" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C10" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D10" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E10" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="82" t="s">
+      <c r="F10" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="82" t="s">
+      <c r="G10" s="80"/>
+      <c r="H10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="82" t="s">
+      <c r="I10" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="82" t="s">
+      <c r="J10" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="82" t="s">
+      <c r="K10" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="K8" s="82" t="s">
+      <c r="L10" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-    </row>
-    <row r="9" spans="1:55" ht="15" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-    </row>
-    <row r="10" spans="1:55" ht="15" customHeight="1">
-      <c r="A10" s="1">
-        <v>1991</v>
-      </c>
-      <c r="B10" s="10">
-        <v>114309</v>
-      </c>
-      <c r="C10" s="10">
-        <v>12335739.900000002</v>
-      </c>
-      <c r="D10" s="10">
-        <v>372990</v>
-      </c>
-      <c r="E10" s="80">
-        <v>3551065.3197163711</v>
-      </c>
-      <c r="F10" s="78">
-        <v>3696236.0420941683</v>
-      </c>
-      <c r="G10" s="7">
-        <f>B10/$B$10</f>
-        <v>1</v>
-      </c>
-      <c r="H10" s="7">
-        <f>C10/$C$10</f>
-        <v>1</v>
-      </c>
-      <c r="I10" s="7">
-        <f>D10/$D$10</f>
-        <v>1</v>
-      </c>
-      <c r="J10" s="79">
-        <f>E10/$E$10</f>
-        <v>1</v>
-      </c>
-      <c r="K10" s="18">
-        <f>F10/$F$10</f>
-        <v>1</v>
-      </c>
-      <c r="M10" s="15"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
@@ -4808,47 +4891,23 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
-    </row>
-    <row r="11" spans="1:55" ht="15" customHeight="1">
-      <c r="A11" s="1">
-        <v>1992</v>
-      </c>
-      <c r="B11" s="10">
-        <v>119168</v>
-      </c>
-      <c r="C11" s="10">
-        <v>12241009.852500003</v>
-      </c>
-      <c r="D11" s="10">
-        <v>383688</v>
-      </c>
-      <c r="E11" s="80">
-        <v>3677039.9671854931</v>
-      </c>
-      <c r="F11" s="78">
-        <v>3828446.0021867193</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" ref="G11:G30" si="0">B11/$B$10</f>
-        <v>1.0425075890787252</v>
-      </c>
-      <c r="H11" s="7">
-        <f t="shared" ref="H11:H30" si="1">C11/$C$10</f>
-        <v>0.9923206837799815</v>
-      </c>
-      <c r="I11" s="7">
-        <f t="shared" ref="I11:I30" si="2">D11/$D$10</f>
-        <v>1.0286817340947478</v>
-      </c>
-      <c r="J11" s="79">
-        <f>E11/$E$10</f>
-        <v>1.0354751704424248</v>
-      </c>
-      <c r="K11" s="18">
-        <f t="shared" ref="K11:K30" si="3">F11/$F$10</f>
-        <v>1.0357688087521719</v>
-      </c>
-      <c r="M11" s="15"/>
+      <c r="AA10" s="15"/>
+    </row>
+    <row r="11" spans="1:56" ht="15" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="83"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
       <c r="P11" s="15"/>
@@ -4862,47 +4921,51 @@
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
-    </row>
-    <row r="12" spans="1:55" ht="15" customHeight="1">
+      <c r="AA11" s="15"/>
+    </row>
+    <row r="12" spans="1:56" ht="15" customHeight="1">
       <c r="A12" s="1">
-        <v>1993</v>
-      </c>
-      <c r="B12" s="10">
-        <v>117290</v>
-      </c>
-      <c r="C12" s="10">
-        <v>12654192.969600003</v>
-      </c>
-      <c r="D12" s="10">
-        <v>389842</v>
-      </c>
-      <c r="E12" s="80">
-        <v>3794592.2455356945</v>
-      </c>
-      <c r="F12" s="78">
-        <v>3950973.580457726</v>
-      </c>
-      <c r="G12" s="7">
-        <f t="shared" si="0"/>
-        <v>1.0260784365185593</v>
+        <v>1991</v>
+      </c>
+      <c r="B12" s="93">
+        <v>114309</v>
+      </c>
+      <c r="C12" s="93">
+        <v>12335739.900000002</v>
+      </c>
+      <c r="D12" s="93">
+        <v>372990</v>
+      </c>
+      <c r="E12" s="93">
+        <v>3551065.3197163711</v>
+      </c>
+      <c r="F12" s="93">
+        <v>3696236.0420941683</v>
+      </c>
+      <c r="G12" s="93">
+        <f>A12-$A$12</f>
+        <v>0</v>
       </c>
       <c r="H12" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0258154818585306</v>
+        <f>B12/$B$12</f>
+        <v>1</v>
       </c>
       <c r="I12" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0451808359473445</v>
-      </c>
-      <c r="J12" s="79">
-        <f>E12/$E$10</f>
-        <v>1.0685785542910753</v>
-      </c>
-      <c r="K12" s="18">
-        <f t="shared" si="3"/>
-        <v>1.0689180927469208</v>
-      </c>
-      <c r="M12" s="15"/>
+        <f>C12/$C$12</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
+        <f>D12/$D$12</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="78">
+        <f t="shared" ref="K12:K32" si="0">E12/$E$12</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="18">
+        <f>F12/$F$12</f>
+        <v>1</v>
+      </c>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
       <c r="P12" s="15"/>
@@ -4916,47 +4979,51 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
       <c r="Z12" s="15"/>
-    </row>
-    <row r="13" spans="1:55" ht="15" customHeight="1">
+      <c r="AA12" s="15"/>
+    </row>
+    <row r="13" spans="1:56" ht="15" customHeight="1">
       <c r="A13" s="1">
-        <v>1994</v>
-      </c>
-      <c r="B13" s="10">
-        <v>116879</v>
-      </c>
-      <c r="C13" s="10">
-        <v>12737954.673000002</v>
-      </c>
-      <c r="D13" s="10">
-        <v>390873</v>
-      </c>
-      <c r="E13" s="80">
-        <v>4036807.1698509222</v>
-      </c>
-      <c r="F13" s="78">
-        <v>4205154.7329356577</v>
-      </c>
-      <c r="G13" s="7">
+        <v>1992</v>
+      </c>
+      <c r="B13" s="93">
+        <v>119168</v>
+      </c>
+      <c r="C13" s="93">
+        <v>12241009.852500003</v>
+      </c>
+      <c r="D13" s="93">
+        <v>383688</v>
+      </c>
+      <c r="E13" s="93">
+        <v>3677039.9671854931</v>
+      </c>
+      <c r="F13" s="93">
+        <v>3828446.0021867193</v>
+      </c>
+      <c r="G13" s="93">
+        <f t="shared" ref="G13:G32" si="1">A13-$A$12</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" ref="H13:H32" si="2">B13/$B$12</f>
+        <v>1.0425075890787252</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" ref="I13:I32" si="3">C13/$C$12</f>
+        <v>0.9923206837799815</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" ref="J13:J32" si="4">D13/$D$12</f>
+        <v>1.0286817340947478</v>
+      </c>
+      <c r="K13" s="78">
         <f t="shared" si="0"/>
-        <v>1.0224829191052323</v>
-      </c>
-      <c r="H13" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0326056463787794</v>
-      </c>
-      <c r="I13" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0479449851202445</v>
-      </c>
-      <c r="J13" s="79">
-        <f>E13/$E$10</f>
-        <v>1.1367876415670517</v>
-      </c>
-      <c r="K13" s="18">
-        <f t="shared" si="3"/>
-        <v>1.1376856578004559</v>
-      </c>
-      <c r="M13" s="15"/>
+        <v>1.0354751704424248</v>
+      </c>
+      <c r="L13" s="18">
+        <f t="shared" ref="L13:L32" si="5">F13/$F$12</f>
+        <v>1.0357688087521719</v>
+      </c>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
@@ -4970,47 +5037,51 @@
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
-    </row>
-    <row r="14" spans="1:55" ht="15" customHeight="1">
+      <c r="AA13" s="15"/>
+    </row>
+    <row r="14" spans="1:56" ht="15" customHeight="1">
       <c r="A14" s="1">
-        <v>1995</v>
-      </c>
-      <c r="B14" s="10">
-        <v>119979</v>
-      </c>
-      <c r="C14" s="10">
-        <v>13170467.925600002</v>
-      </c>
-      <c r="D14" s="10">
-        <v>390546</v>
-      </c>
-      <c r="E14" s="80">
-        <v>4188241.2731711413</v>
-      </c>
-      <c r="F14" s="78">
-        <v>4360522.0557862297</v>
-      </c>
-      <c r="G14" s="7">
+        <v>1993</v>
+      </c>
+      <c r="B14" s="93">
+        <v>117290</v>
+      </c>
+      <c r="C14" s="93">
+        <v>12654192.969600003</v>
+      </c>
+      <c r="D14" s="93">
+        <v>389842</v>
+      </c>
+      <c r="E14" s="93">
+        <v>3794592.2455356945</v>
+      </c>
+      <c r="F14" s="93">
+        <v>3950973.580457726</v>
+      </c>
+      <c r="G14" s="93">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0260784365185593</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="3"/>
+        <v>1.0258154818585306</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="4"/>
+        <v>1.0451808359473445</v>
+      </c>
+      <c r="K14" s="78">
         <f t="shared" si="0"/>
-        <v>1.0496023935123218</v>
-      </c>
-      <c r="H14" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0676674469765692</v>
-      </c>
-      <c r="I14" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0470682860130298</v>
-      </c>
-      <c r="J14" s="79">
-        <f>E14/$E$10</f>
-        <v>1.1794323382104563</v>
-      </c>
-      <c r="K14" s="18">
-        <f t="shared" si="3"/>
-        <v>1.1797195866624628</v>
-      </c>
-      <c r="M14" s="15"/>
+        <v>1.0685785542910753</v>
+      </c>
+      <c r="L14" s="18">
+        <f t="shared" si="5"/>
+        <v>1.0689180927469208</v>
+      </c>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
@@ -5024,47 +5095,51 @@
       <c r="X14" s="15"/>
       <c r="Y14" s="15"/>
       <c r="Z14" s="15"/>
-    </row>
-    <row r="15" spans="1:55" ht="15" customHeight="1">
+      <c r="AA14" s="15"/>
+    </row>
+    <row r="15" spans="1:56" ht="15" customHeight="1">
       <c r="A15" s="1">
-        <v>1996</v>
-      </c>
-      <c r="B15" s="10">
-        <v>128499</v>
-      </c>
-      <c r="C15" s="10">
-        <v>13276064.253800001</v>
-      </c>
-      <c r="D15" s="10">
-        <v>397008</v>
-      </c>
-      <c r="E15" s="80">
-        <v>4338410.1102254707</v>
-      </c>
-      <c r="F15" s="78">
-        <v>4514440.1933225989</v>
-      </c>
-      <c r="G15" s="7">
+        <v>1994</v>
+      </c>
+      <c r="B15" s="93">
+        <v>116879</v>
+      </c>
+      <c r="C15" s="93">
+        <v>12737954.673000002</v>
+      </c>
+      <c r="D15" s="93">
+        <v>390873</v>
+      </c>
+      <c r="E15" s="93">
+        <v>4036807.1698509222</v>
+      </c>
+      <c r="F15" s="93">
+        <v>4205154.7329356577</v>
+      </c>
+      <c r="G15" s="93">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0224829191052323</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="3"/>
+        <v>1.0326056463787794</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="4"/>
+        <v>1.0479449851202445</v>
+      </c>
+      <c r="K15" s="78">
         <f t="shared" si="0"/>
-        <v>1.1241372070440647</v>
-      </c>
-      <c r="H15" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0762276410999878</v>
-      </c>
-      <c r="I15" s="7">
-        <f t="shared" si="2"/>
-        <v>1.0643931472693637</v>
-      </c>
-      <c r="J15" s="79">
-        <f>E15/$E$10</f>
-        <v>1.2217207287451377</v>
-      </c>
-      <c r="K15" s="18">
-        <f t="shared" si="3"/>
-        <v>1.2213614449700736</v>
-      </c>
-      <c r="M15" s="15"/>
+        <v>1.1367876415670517</v>
+      </c>
+      <c r="L15" s="18">
+        <f t="shared" si="5"/>
+        <v>1.1376856578004559</v>
+      </c>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
@@ -5078,47 +5153,51 @@
       <c r="X15" s="15"/>
       <c r="Y15" s="15"/>
       <c r="Z15" s="15"/>
-    </row>
-    <row r="16" spans="1:55" ht="15" customHeight="1">
+      <c r="AA15" s="15"/>
+    </row>
+    <row r="16" spans="1:56" ht="15" customHeight="1">
       <c r="A16" s="1">
-        <v>1997</v>
-      </c>
-      <c r="B16" s="10">
-        <v>132848</v>
-      </c>
-      <c r="C16" s="10">
-        <v>14125906.439999999</v>
-      </c>
-      <c r="D16" s="10">
-        <v>407239</v>
-      </c>
-      <c r="E16" s="80">
-        <v>4846438.8975911848</v>
-      </c>
-      <c r="F16" s="78">
-        <v>5045596.2747649644</v>
-      </c>
-      <c r="G16" s="7">
+        <v>1995</v>
+      </c>
+      <c r="B16" s="93">
+        <v>119979</v>
+      </c>
+      <c r="C16" s="93">
+        <v>13170467.925600002</v>
+      </c>
+      <c r="D16" s="93">
+        <v>390546</v>
+      </c>
+      <c r="E16" s="93">
+        <v>4188241.2731711413</v>
+      </c>
+      <c r="F16" s="93">
+        <v>4360522.0557862297</v>
+      </c>
+      <c r="G16" s="93">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0496023935123218</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="3"/>
+        <v>1.0676674469765692</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="4"/>
+        <v>1.0470682860130298</v>
+      </c>
+      <c r="K16" s="78">
         <f t="shared" si="0"/>
-        <v>1.1621832051719463</v>
-      </c>
-      <c r="H16" s="7">
-        <f t="shared" si="1"/>
-        <v>1.1451203214814862</v>
-      </c>
-      <c r="I16" s="7">
-        <f t="shared" si="2"/>
-        <v>1.09182283707338</v>
-      </c>
-      <c r="J16" s="79">
-        <f>E16/$E$10</f>
-        <v>1.3647844973964818</v>
-      </c>
-      <c r="K16" s="18">
-        <f t="shared" si="3"/>
-        <v>1.3650633285601241</v>
-      </c>
-      <c r="M16" s="15"/>
+        <v>1.1794323382104563</v>
+      </c>
+      <c r="L16" s="18">
+        <f t="shared" si="5"/>
+        <v>1.1797195866624628</v>
+      </c>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
@@ -5132,623 +5211,1383 @@
       <c r="X16" s="15"/>
       <c r="Y16" s="15"/>
       <c r="Z16" s="15"/>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1">
+      <c r="AA16" s="15"/>
+    </row>
+    <row r="17" spans="1:27" ht="15" customHeight="1">
       <c r="A17" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B17" s="93">
+        <v>128499</v>
+      </c>
+      <c r="C17" s="93">
+        <v>13276064.253800001</v>
+      </c>
+      <c r="D17" s="93">
+        <v>397008</v>
+      </c>
+      <c r="E17" s="93">
+        <v>4338410.1102254707</v>
+      </c>
+      <c r="F17" s="93">
+        <v>4514440.1933225989</v>
+      </c>
+      <c r="G17" s="93">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1241372070440647</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="3"/>
+        <v>1.0762276410999878</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="4"/>
+        <v>1.0643931472693637</v>
+      </c>
+      <c r="K17" s="78">
+        <f t="shared" si="0"/>
+        <v>1.2217207287451377</v>
+      </c>
+      <c r="L17" s="18">
+        <f t="shared" si="5"/>
+        <v>1.2213614449700736</v>
+      </c>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+    </row>
+    <row r="18" spans="1:27" ht="15" customHeight="1">
+      <c r="A18" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B18" s="93">
+        <v>132848</v>
+      </c>
+      <c r="C18" s="93">
+        <v>14125906.439999999</v>
+      </c>
+      <c r="D18" s="93">
+        <v>407239</v>
+      </c>
+      <c r="E18" s="93">
+        <v>4846438.8975911848</v>
+      </c>
+      <c r="F18" s="93">
+        <v>5045596.2747649644</v>
+      </c>
+      <c r="G18" s="93">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1621832051719463</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="3"/>
+        <v>1.1451203214814862</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="4"/>
+        <v>1.09182283707338</v>
+      </c>
+      <c r="K18" s="78">
+        <f t="shared" si="0"/>
+        <v>1.3647844973964818</v>
+      </c>
+      <c r="L18" s="18">
+        <f t="shared" si="5"/>
+        <v>1.3650633285601241</v>
+      </c>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+    </row>
+    <row r="19" spans="1:27" ht="15" customHeight="1">
+      <c r="A19" s="1">
         <v>1998</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B19" s="93">
         <v>136489</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C19" s="93">
         <v>14874142.339199997</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D19" s="93">
         <v>417988</v>
       </c>
-      <c r="E17" s="80">
+      <c r="E19" s="93">
         <v>5026099.8891465338</v>
       </c>
-      <c r="F17" s="78">
+      <c r="F19" s="93">
         <v>5228082.7618776634</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G19" s="93">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H19" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1940354652739504</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="3"/>
+        <v>1.2057762614790537</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="4"/>
+        <v>1.1206413040564089</v>
+      </c>
+      <c r="K19" s="78">
         <f t="shared" si="0"/>
-        <v>1.1940354652739504</v>
-      </c>
-      <c r="H17" s="7">
+        <v>1.4153780447913518</v>
+      </c>
+      <c r="L19" s="18">
+        <f t="shared" si="5"/>
+        <v>1.4144342250706479</v>
+      </c>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:27" ht="15" customHeight="1">
+      <c r="A20" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B20" s="93">
+        <v>139129</v>
+      </c>
+      <c r="C20" s="93">
+        <v>15388226.695800001</v>
+      </c>
+      <c r="D20" s="93">
+        <v>430264</v>
+      </c>
+      <c r="E20" s="93">
+        <v>5300745.3919546278</v>
+      </c>
+      <c r="F20" s="93">
+        <v>5510665.7264289036</v>
+      </c>
+      <c r="G20" s="93">
         <f t="shared" si="1"/>
-        <v>1.2057762614790537</v>
-      </c>
-      <c r="I17" s="7">
+        <v>8</v>
+      </c>
+      <c r="H20" s="7">
         <f t="shared" si="2"/>
-        <v>1.1206413040564089</v>
-      </c>
-      <c r="J17" s="79">
-        <f>E17/$E$10</f>
-        <v>1.4153780447913518</v>
-      </c>
-      <c r="K17" s="18">
+        <v>1.2171307596077299</v>
+      </c>
+      <c r="I20" s="7">
         <f t="shared" si="3"/>
-        <v>1.4144342250706479</v>
-      </c>
-      <c r="M17" s="15"/>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
-      <c r="A18" s="1">
-        <v>1999</v>
-      </c>
-      <c r="B18" s="10">
-        <v>139129</v>
-      </c>
-      <c r="C18" s="10">
-        <v>15388226.695800001</v>
-      </c>
-      <c r="D18" s="10">
-        <v>430264</v>
-      </c>
-      <c r="E18" s="80">
-        <v>5300745.3919546278</v>
-      </c>
-      <c r="F18" s="78">
-        <v>5510665.7264289036</v>
-      </c>
-      <c r="G18" s="7">
+        <v>1.2474506450804785</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="4"/>
+        <v>1.1535537145767982</v>
+      </c>
+      <c r="K20" s="78">
         <f t="shared" si="0"/>
-        <v>1.2171307596077299</v>
-      </c>
-      <c r="H18" s="7">
+        <v>1.4927197656780942</v>
+      </c>
+      <c r="L20" s="18">
+        <f t="shared" si="5"/>
+        <v>1.4908857723563396</v>
+      </c>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:27" ht="15" customHeight="1">
+      <c r="A21" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B21" s="93">
+        <v>146284</v>
+      </c>
+      <c r="C21" s="93">
+        <v>16564277.866500001</v>
+      </c>
+      <c r="D21" s="93">
+        <v>443388</v>
+      </c>
+      <c r="E21" s="93">
+        <v>5518209.5422440665</v>
+      </c>
+      <c r="F21" s="93">
+        <v>5733164.209871687</v>
+      </c>
+      <c r="G21" s="93">
         <f t="shared" si="1"/>
-        <v>1.2474506450804785</v>
-      </c>
-      <c r="I18" s="7">
+        <v>9</v>
+      </c>
+      <c r="H21" s="7">
         <f t="shared" si="2"/>
-        <v>1.1535537145767982</v>
-      </c>
-      <c r="J18" s="79">
-        <f>E18/$E$10</f>
-        <v>1.4927197656780942</v>
-      </c>
-      <c r="K18" s="18">
+        <v>1.2797242561828028</v>
+      </c>
+      <c r="I21" s="7">
         <f t="shared" si="3"/>
-        <v>1.4908857723563396</v>
-      </c>
-      <c r="M18" s="15"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1">
-      <c r="A19" s="1">
-        <v>2000</v>
-      </c>
-      <c r="B19" s="10">
-        <v>146284</v>
-      </c>
-      <c r="C19" s="10">
-        <v>16564277.866500001</v>
-      </c>
-      <c r="D19" s="10">
-        <v>443388</v>
-      </c>
-      <c r="E19" s="80">
-        <v>5518209.5422440665</v>
-      </c>
-      <c r="F19" s="78">
-        <v>5733164.209871687</v>
-      </c>
-      <c r="G19" s="7">
+        <v>1.3427875426021263</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="4"/>
+        <v>1.1887396444944904</v>
+      </c>
+      <c r="K21" s="78">
         <f t="shared" si="0"/>
-        <v>1.2797242561828028</v>
-      </c>
-      <c r="H19" s="7">
+        <v>1.5539588955476646</v>
+      </c>
+      <c r="L21" s="18">
+        <f t="shared" si="5"/>
+        <v>1.5510817341155141</v>
+      </c>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:27" ht="15" customHeight="1">
+      <c r="A22" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B22" s="93">
+        <v>151652</v>
+      </c>
+      <c r="C22" s="93">
+        <v>17327731.398899999</v>
+      </c>
+      <c r="D22" s="93">
+        <v>461719</v>
+      </c>
+      <c r="E22" s="93">
+        <v>5902028.7403752711</v>
+      </c>
+      <c r="F22" s="93">
+        <v>6129476.8397576045</v>
+      </c>
+      <c r="G22" s="93">
         <f t="shared" si="1"/>
-        <v>1.3427875426021263</v>
-      </c>
-      <c r="I19" s="7">
+        <v>10</v>
+      </c>
+      <c r="H22" s="7">
         <f t="shared" si="2"/>
-        <v>1.1887396444944904</v>
-      </c>
-      <c r="J19" s="79">
-        <f>E19/$E$10</f>
-        <v>1.5539588955476646</v>
-      </c>
-      <c r="K19" s="18">
+        <v>1.3266846879948211</v>
+      </c>
+      <c r="I22" s="7">
         <f t="shared" si="3"/>
-        <v>1.5510817341155141</v>
-      </c>
-      <c r="M19" s="15"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1">
-      <c r="A20" s="1">
-        <v>2001</v>
-      </c>
-      <c r="B20" s="10">
-        <v>151652</v>
-      </c>
-      <c r="C20" s="10">
-        <v>17327731.398899999</v>
-      </c>
-      <c r="D20" s="10">
-        <v>461719</v>
-      </c>
-      <c r="E20" s="80">
-        <v>5902028.7403752711</v>
-      </c>
-      <c r="F20" s="78">
-        <v>6129476.8397576045</v>
-      </c>
-      <c r="G20" s="7">
+        <v>1.4046771040381612</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="4"/>
+        <v>1.2378857342019893</v>
+      </c>
+      <c r="K22" s="78">
         <f t="shared" si="0"/>
-        <v>1.3266846879948211</v>
-      </c>
-      <c r="H20" s="7">
+        <v>1.6620445440994238</v>
+      </c>
+      <c r="L22" s="18">
+        <f t="shared" si="5"/>
+        <v>1.6583023297085866</v>
+      </c>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:27" ht="15" customHeight="1">
+      <c r="A23" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B23" s="93">
+        <v>163050</v>
+      </c>
+      <c r="C23" s="93">
+        <v>18086977.934999999</v>
+      </c>
+      <c r="D23" s="93">
+        <v>484696</v>
+      </c>
+      <c r="E23" s="93">
+        <v>6444915.7124548433</v>
+      </c>
+      <c r="F23" s="93">
+        <v>6693245.7696196595</v>
+      </c>
+      <c r="G23" s="93">
         <f t="shared" si="1"/>
-        <v>1.4046771040381612</v>
-      </c>
-      <c r="I20" s="7">
+        <v>11</v>
+      </c>
+      <c r="H23" s="7">
         <f t="shared" si="2"/>
-        <v>1.2378857342019893</v>
-      </c>
-      <c r="J20" s="79">
-        <f>E20/$E$10</f>
-        <v>1.6620445440994238</v>
-      </c>
-      <c r="K20" s="18">
+        <v>1.4263968716374038</v>
+      </c>
+      <c r="I23" s="7">
         <f t="shared" si="3"/>
-        <v>1.6583023297085866</v>
-      </c>
-      <c r="M20" s="15"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1">
-      <c r="A21" s="1">
-        <v>2002</v>
-      </c>
-      <c r="B21" s="10">
-        <v>163050</v>
-      </c>
-      <c r="C21" s="10">
-        <v>18086977.934999999</v>
-      </c>
-      <c r="D21" s="10">
-        <v>484696</v>
-      </c>
-      <c r="E21" s="80">
-        <v>6444915.7124548433</v>
-      </c>
-      <c r="F21" s="78">
-        <v>6693245.7696196595</v>
-      </c>
-      <c r="G21" s="7">
+        <v>1.4662256242124556</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="4"/>
+        <v>1.2994879219282018</v>
+      </c>
+      <c r="K23" s="78">
         <f t="shared" si="0"/>
-        <v>1.4263968716374038</v>
-      </c>
-      <c r="H21" s="7">
+        <v>1.8149245739499966</v>
+      </c>
+      <c r="L23" s="18">
+        <f t="shared" si="5"/>
+        <v>1.8108274724325999</v>
+      </c>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:27" ht="15" customHeight="1">
+      <c r="A24" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B24" s="93">
+        <v>174650</v>
+      </c>
+      <c r="C24" s="93">
+        <v>19329521.379999999</v>
+      </c>
+      <c r="D24" s="93">
+        <v>512030</v>
+      </c>
+      <c r="E24" s="93">
+        <v>6783911.9365747431</v>
+      </c>
+      <c r="F24" s="93">
+        <v>7042781.0211911267</v>
+      </c>
+      <c r="G24" s="93">
         <f t="shared" si="1"/>
-        <v>1.4662256242124556</v>
-      </c>
-      <c r="I21" s="7">
+        <v>12</v>
+      </c>
+      <c r="H24" s="7">
         <f t="shared" si="2"/>
-        <v>1.2994879219282018</v>
-      </c>
-      <c r="J21" s="79">
-        <f>E21/$E$10</f>
-        <v>1.8149245739499966</v>
-      </c>
-      <c r="K21" s="18">
+        <v>1.5278761952252229</v>
+      </c>
+      <c r="I24" s="7">
         <f t="shared" si="3"/>
-        <v>1.8108274724325999</v>
-      </c>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1">
-      <c r="A22" s="1">
-        <v>2003</v>
-      </c>
-      <c r="B22" s="10">
-        <v>174650</v>
-      </c>
-      <c r="C22" s="10">
-        <v>19329521.379999999</v>
-      </c>
-      <c r="D22" s="10">
-        <v>512030</v>
-      </c>
-      <c r="E22" s="80">
-        <v>6783911.9365747431</v>
-      </c>
-      <c r="F22" s="78">
-        <v>7042781.0211911267</v>
-      </c>
-      <c r="G22" s="7">
+        <v>1.5669527354415114</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="4"/>
+        <v>1.3727713879728678</v>
+      </c>
+      <c r="K24" s="78">
         <f t="shared" si="0"/>
-        <v>1.5278761952252229</v>
-      </c>
-      <c r="H22" s="7">
+        <v>1.9103878204968034</v>
+      </c>
+      <c r="L24" s="18">
+        <f t="shared" si="5"/>
+        <v>1.9053926591768511</v>
+      </c>
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" spans="1:27" ht="15" customHeight="1">
+      <c r="A25" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B25" s="93">
+        <v>183530</v>
+      </c>
+      <c r="C25" s="93">
+        <v>21122692.831799999</v>
+      </c>
+      <c r="D25" s="93">
+        <v>541714</v>
+      </c>
+      <c r="E25" s="93">
+        <v>7050938.73583184</v>
+      </c>
+      <c r="F25" s="93">
+        <v>7314803.0058149267</v>
+      </c>
+      <c r="G25" s="93">
         <f t="shared" si="1"/>
-        <v>1.5669527354415114</v>
-      </c>
-      <c r="I22" s="7">
+        <v>13</v>
+      </c>
+      <c r="H25" s="7">
         <f t="shared" si="2"/>
-        <v>1.3727713879728678</v>
-      </c>
-      <c r="J22" s="79">
-        <f>E22/$E$10</f>
-        <v>1.9103878204968034</v>
-      </c>
-      <c r="K22" s="18">
+        <v>1.6055603670752083</v>
+      </c>
+      <c r="I25" s="7">
         <f t="shared" si="3"/>
-        <v>1.9053926591768511</v>
-      </c>
-      <c r="M22" s="15"/>
-    </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1">
-      <c r="A23" s="1">
-        <v>2004</v>
-      </c>
-      <c r="B23" s="10">
-        <v>183530</v>
-      </c>
-      <c r="C23" s="10">
-        <v>21122692.831799999</v>
-      </c>
-      <c r="D23" s="10">
-        <v>541714</v>
-      </c>
-      <c r="E23" s="80">
-        <v>7050938.73583184</v>
-      </c>
-      <c r="F23" s="78">
-        <v>7314803.0058149267</v>
-      </c>
-      <c r="G23" s="7">
+        <v>1.7123166508885288</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="4"/>
+        <v>1.4523552910265691</v>
+      </c>
+      <c r="K25" s="78">
         <f t="shared" si="0"/>
-        <v>1.6055603670752083</v>
-      </c>
-      <c r="H23" s="7">
+        <v>1.9855840715413844</v>
+      </c>
+      <c r="L25" s="18">
+        <f t="shared" si="5"/>
+        <v>1.978986980947947</v>
+      </c>
+      <c r="N25" s="15"/>
+    </row>
+    <row r="26" spans="1:27" ht="15" customHeight="1">
+      <c r="A26" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B26" s="93">
+        <v>192015</v>
+      </c>
+      <c r="C26" s="93">
+        <v>21672707.775600001</v>
+      </c>
+      <c r="D26" s="93">
+        <v>572644</v>
+      </c>
+      <c r="E26" s="93">
+        <v>8042709.2271035835</v>
+      </c>
+      <c r="F26" s="93">
+        <v>8346190.4671160309</v>
+      </c>
+      <c r="G26" s="93">
         <f t="shared" si="1"/>
-        <v>1.7123166508885288</v>
-      </c>
-      <c r="I23" s="7">
+        <v>14</v>
+      </c>
+      <c r="H26" s="7">
         <f t="shared" si="2"/>
-        <v>1.4523552910265691</v>
-      </c>
-      <c r="J23" s="79">
-        <f>E23/$E$10</f>
-        <v>1.9855840715413844</v>
-      </c>
-      <c r="K23" s="18">
+        <v>1.6797889929926777</v>
+      </c>
+      <c r="I26" s="7">
         <f t="shared" si="3"/>
-        <v>1.978986980947947</v>
-      </c>
-      <c r="M23" s="15"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1">
-      <c r="A24" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B24" s="10">
-        <v>192015</v>
-      </c>
-      <c r="C24" s="10">
-        <v>21672707.775600001</v>
-      </c>
-      <c r="D24" s="10">
-        <v>572644</v>
-      </c>
-      <c r="E24" s="80">
-        <v>8042709.2271035835</v>
-      </c>
-      <c r="F24" s="78">
-        <v>8346190.4671160309</v>
-      </c>
-      <c r="G24" s="7">
+        <v>1.7569037569931252</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="4"/>
+        <v>1.5352797662135713</v>
+      </c>
+      <c r="K26" s="78">
         <f t="shared" si="0"/>
-        <v>1.6797889929926777</v>
-      </c>
-      <c r="H24" s="7">
+        <v>2.264872229313418</v>
+      </c>
+      <c r="L26" s="18">
+        <f t="shared" si="5"/>
+        <v>2.2580242095110754</v>
+      </c>
+      <c r="N26" s="15"/>
+    </row>
+    <row r="27" spans="1:27" ht="15" customHeight="1">
+      <c r="A27" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B27" s="93">
+        <v>203332</v>
+      </c>
+      <c r="C27" s="93">
+        <v>21703991.445</v>
+      </c>
+      <c r="D27" s="93">
+        <v>603700</v>
+      </c>
+      <c r="E27" s="93">
+        <v>8404315.8856006898</v>
+      </c>
+      <c r="F27" s="93">
+        <v>8727267.6872208156</v>
+      </c>
+      <c r="G27" s="93">
         <f t="shared" si="1"/>
-        <v>1.7569037569931252</v>
-      </c>
-      <c r="I24" s="7">
+        <v>15</v>
+      </c>
+      <c r="H27" s="7">
         <f t="shared" si="2"/>
-        <v>1.5352797662135713</v>
-      </c>
-      <c r="J24" s="79">
-        <f>E24/$E$10</f>
-        <v>2.264872229313418</v>
-      </c>
-      <c r="K24" s="18">
+        <v>1.7787925710136561</v>
+      </c>
+      <c r="I27" s="7">
         <f t="shared" si="3"/>
-        <v>2.2580242095110754</v>
-      </c>
-      <c r="M24" s="15"/>
-    </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1">
-      <c r="A25" s="1">
-        <v>2006</v>
-      </c>
-      <c r="B25" s="10">
-        <v>203332</v>
-      </c>
-      <c r="C25" s="10">
-        <v>21703991.445</v>
-      </c>
-      <c r="D25" s="10">
-        <v>603700</v>
-      </c>
-      <c r="E25" s="80">
-        <v>8404315.8856006898</v>
-      </c>
-      <c r="F25" s="78">
-        <v>8727267.6872208156</v>
-      </c>
-      <c r="G25" s="7">
+        <v>1.7594397758824338</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="4"/>
+        <v>1.618542052065739</v>
+      </c>
+      <c r="K27" s="78">
         <f t="shared" si="0"/>
-        <v>1.7787925710136561</v>
-      </c>
-      <c r="H25" s="7">
+        <v>2.3667027015633595</v>
+      </c>
+      <c r="L27" s="18">
+        <f t="shared" si="5"/>
+        <v>2.3611229336631401</v>
+      </c>
+      <c r="N27" s="15"/>
+    </row>
+    <row r="28" spans="1:27" ht="15" customHeight="1">
+      <c r="A28" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B28" s="93">
+        <v>219242</v>
+      </c>
+      <c r="C28" s="93">
+        <v>22259301.176800001</v>
+      </c>
+      <c r="D28" s="93">
+        <v>636848</v>
+      </c>
+      <c r="E28" s="93">
+        <v>8611730.9580265898</v>
+      </c>
+      <c r="F28" s="93">
+        <v>8940922.2509191744</v>
+      </c>
+      <c r="G28" s="93">
         <f t="shared" si="1"/>
-        <v>1.7594397758824338</v>
-      </c>
-      <c r="I25" s="7">
+        <v>16</v>
+      </c>
+      <c r="H28" s="7">
         <f t="shared" si="2"/>
-        <v>1.618542052065739</v>
-      </c>
-      <c r="J25" s="79">
-        <f>E25/$E$10</f>
-        <v>2.3667027015633595</v>
-      </c>
-      <c r="K25" s="18">
+        <v>1.9179767122448801</v>
+      </c>
+      <c r="I28" s="7">
         <f t="shared" si="3"/>
-        <v>2.3611229336631401</v>
-      </c>
-      <c r="M25" s="15"/>
-    </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1">
-      <c r="A26" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B26" s="10">
-        <v>219242</v>
-      </c>
-      <c r="C26" s="10">
-        <v>22259301.176800001</v>
-      </c>
-      <c r="D26" s="10">
-        <v>636848</v>
-      </c>
-      <c r="E26" s="80">
-        <v>8611730.9580265898</v>
-      </c>
-      <c r="F26" s="78">
-        <v>8940922.2509191744</v>
-      </c>
-      <c r="G26" s="7">
+        <v>1.8044561053690826</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="4"/>
+        <v>1.7074130673744605</v>
+      </c>
+      <c r="K28" s="78">
         <f t="shared" si="0"/>
-        <v>1.9179767122448801</v>
-      </c>
-      <c r="H26" s="7">
+        <v>2.42511195449213</v>
+      </c>
+      <c r="L28" s="18">
+        <f t="shared" si="5"/>
+        <v>2.4189262128003968</v>
+      </c>
+      <c r="N28" s="15"/>
+    </row>
+    <row r="29" spans="1:27" ht="15" customHeight="1">
+      <c r="A29" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B29" s="93">
+        <v>224285</v>
+      </c>
+      <c r="C29" s="93">
+        <v>21426545.852400001</v>
+      </c>
+      <c r="D29" s="93">
+        <v>671446</v>
+      </c>
+      <c r="E29" s="93">
+        <v>8871291.8524665684</v>
+      </c>
+      <c r="F29" s="93">
+        <v>9225872.4011120647</v>
+      </c>
+      <c r="G29" s="93">
         <f t="shared" si="1"/>
-        <v>1.8044561053690826</v>
-      </c>
-      <c r="I26" s="7">
+        <v>17</v>
+      </c>
+      <c r="H29" s="7">
         <f t="shared" si="2"/>
-        <v>1.7074130673744605</v>
-      </c>
-      <c r="J26" s="79">
-        <f>E26/$E$10</f>
-        <v>2.42511195449213</v>
-      </c>
-      <c r="K26" s="18">
+        <v>1.9620939733529292</v>
+      </c>
+      <c r="I29" s="7">
         <f t="shared" si="3"/>
-        <v>2.4189262128003968</v>
-      </c>
-      <c r="M26" s="15"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1">
-      <c r="A27" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B27" s="10">
-        <v>224285</v>
-      </c>
-      <c r="C27" s="10">
-        <v>21426545.852400001</v>
-      </c>
-      <c r="D27" s="10">
-        <v>671446</v>
-      </c>
-      <c r="E27" s="80">
-        <v>8871291.8524665684</v>
-      </c>
-      <c r="F27" s="78">
-        <v>9225872.4011120647</v>
-      </c>
-      <c r="G27" s="7">
+        <v>1.7369485759342249</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="4"/>
+        <v>1.8001715863696077</v>
+      </c>
+      <c r="K29" s="78">
         <f t="shared" si="0"/>
-        <v>1.9620939733529292</v>
-      </c>
-      <c r="H27" s="7">
+        <v>2.498205764678846</v>
+      </c>
+      <c r="L29" s="18">
+        <f t="shared" si="5"/>
+        <v>2.4960181914910886</v>
+      </c>
+      <c r="N29" s="15"/>
+    </row>
+    <row r="30" spans="1:27" ht="15" customHeight="1">
+      <c r="A30" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B30" s="93">
+        <v>228322</v>
+      </c>
+      <c r="C30" s="93">
+        <v>21963085.544399999</v>
+      </c>
+      <c r="D30" s="93">
+        <v>706393</v>
+      </c>
+      <c r="E30" s="93">
+        <v>9868533.3309457917</v>
+      </c>
+      <c r="F30" s="93">
+        <v>10261819.072992271</v>
+      </c>
+      <c r="G30" s="93">
         <f t="shared" si="1"/>
-        <v>1.7369485759342249</v>
-      </c>
-      <c r="I27" s="7">
+        <v>18</v>
+      </c>
+      <c r="H30" s="7">
         <f t="shared" si="2"/>
-        <v>1.8001715863696077</v>
-      </c>
-      <c r="J27" s="79">
-        <f>E27/$E$10</f>
-        <v>2.498205764678846</v>
-      </c>
-      <c r="K27" s="18">
+        <v>1.9974105276050005</v>
+      </c>
+      <c r="I30" s="7">
         <f t="shared" si="3"/>
-        <v>2.4960181914910886</v>
-      </c>
-      <c r="M27" s="15"/>
-    </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1">
-      <c r="A28" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B28" s="10">
-        <v>228322</v>
-      </c>
-      <c r="C28" s="10">
-        <v>21963085.544399999</v>
-      </c>
-      <c r="D28" s="10">
-        <v>706393</v>
-      </c>
-      <c r="E28" s="80">
-        <v>9868533.3309457917</v>
-      </c>
-      <c r="F28" s="78">
-        <v>10261819.072992271</v>
-      </c>
-      <c r="G28" s="7">
+        <v>1.7804433072068904</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" si="4"/>
+        <v>1.8938657872865223</v>
+      </c>
+      <c r="K30" s="78">
         <f t="shared" si="0"/>
-        <v>1.9974105276050005</v>
-      </c>
-      <c r="H28" s="7">
+        <v>2.7790345832709171</v>
+      </c>
+      <c r="L30" s="18">
+        <f t="shared" si="5"/>
+        <v>2.7762888939252521</v>
+      </c>
+      <c r="N30" s="15"/>
+    </row>
+    <row r="31" spans="1:27" ht="15" customHeight="1">
+      <c r="A31" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B31" s="93">
+        <v>234966</v>
+      </c>
+      <c r="C31" s="93">
+        <v>22783878.039999999</v>
+      </c>
+      <c r="D31" s="93">
+        <v>741352</v>
+      </c>
+      <c r="E31" s="93">
+        <v>9353591.9376285113</v>
+      </c>
+      <c r="F31" s="93">
+        <v>9698127.466241559</v>
+      </c>
+      <c r="G31" s="93">
         <f t="shared" si="1"/>
-        <v>1.7804433072068904</v>
-      </c>
-      <c r="I28" s="7">
+        <v>19</v>
+      </c>
+      <c r="H31" s="7">
         <f t="shared" si="2"/>
-        <v>1.8938657872865223</v>
-      </c>
-      <c r="J28" s="79">
-        <f>E28/$E$10</f>
-        <v>2.7790345832709171</v>
-      </c>
-      <c r="K28" s="18">
+        <v>2.055533685011679</v>
+      </c>
+      <c r="I31" s="7">
         <f t="shared" si="3"/>
-        <v>2.7762888939252521</v>
-      </c>
-      <c r="M28" s="15"/>
-    </row>
-    <row r="29" spans="1:13" ht="15" customHeight="1">
-      <c r="A29" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B29" s="10">
-        <v>234966</v>
-      </c>
-      <c r="C29" s="10">
-        <v>22783878.039999999</v>
-      </c>
-      <c r="D29" s="10">
-        <v>741352</v>
-      </c>
-      <c r="E29" s="80">
-        <v>9353591.9376285113</v>
-      </c>
-      <c r="F29" s="78">
-        <v>9698127.466241559</v>
-      </c>
-      <c r="G29" s="7">
+        <v>1.8469810667781668</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="4"/>
+        <v>1.9875921606477385</v>
+      </c>
+      <c r="K31" s="78">
         <f t="shared" si="0"/>
-        <v>2.055533685011679</v>
-      </c>
-      <c r="H29" s="7">
+        <v>2.6340241858394191</v>
+      </c>
+      <c r="L31" s="18">
+        <f t="shared" si="5"/>
+        <v>2.6237846706204704</v>
+      </c>
+      <c r="N31" s="15"/>
+    </row>
+    <row r="32" spans="1:27" ht="15" customHeight="1">
+      <c r="A32" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B32" s="93">
+        <v>239718</v>
+      </c>
+      <c r="C32" s="94">
+        <v>23037968.492000002</v>
+      </c>
+      <c r="D32" s="93">
+        <v>778085</v>
+      </c>
+      <c r="E32" s="93">
+        <v>10812471.557392137</v>
+      </c>
+      <c r="F32" s="93">
+        <v>11254432.861191383</v>
+      </c>
+      <c r="G32" s="93">
         <f t="shared" si="1"/>
-        <v>1.8469810667781668</v>
-      </c>
-      <c r="I29" s="7">
+        <v>20</v>
+      </c>
+      <c r="H32" s="7">
         <f t="shared" si="2"/>
-        <v>1.9875921606477385</v>
-      </c>
-      <c r="J29" s="79">
-        <f>E29/$E$10</f>
-        <v>2.6340241858394191</v>
-      </c>
-      <c r="K29" s="18">
+        <v>2.097105214812482</v>
+      </c>
+      <c r="I32" s="7">
         <f t="shared" si="3"/>
-        <v>2.6237846706204704</v>
-      </c>
-      <c r="M29" s="15"/>
-    </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1">
-      <c r="A30" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B30" s="10">
-        <v>239718</v>
-      </c>
-      <c r="C30" s="15">
-        <v>23037968.492000002</v>
-      </c>
-      <c r="D30" s="10">
-        <v>778085</v>
-      </c>
-      <c r="E30" s="80">
-        <v>10812471.557392137</v>
-      </c>
-      <c r="F30" s="80">
-        <v>11254432.861191383</v>
-      </c>
-      <c r="G30" s="7">
+        <v>1.8675789761098966</v>
+      </c>
+      <c r="J32" s="7">
+        <f t="shared" si="4"/>
+        <v>2.0860746936915198</v>
+      </c>
+      <c r="K32" s="78">
         <f t="shared" si="0"/>
-        <v>2.097105214812482</v>
-      </c>
-      <c r="H30" s="7">
-        <f t="shared" si="1"/>
-        <v>1.8675789761098966</v>
-      </c>
-      <c r="I30" s="7">
-        <f t="shared" si="2"/>
-        <v>2.0860746936915198</v>
-      </c>
-      <c r="J30" s="79">
-        <f>E30/$E$10</f>
         <v>3.0448529057910276</v>
       </c>
-      <c r="K30" s="79">
-        <f t="shared" si="3"/>
+      <c r="L32" s="78">
+        <f t="shared" si="5"/>
         <v>3.044836080007213</v>
       </c>
-      <c r="M30" s="15"/>
-    </row>
-    <row r="33" spans="2:24">
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="75"/>
-      <c r="K33" s="75"/>
-      <c r="L33" s="75"/>
-      <c r="M33" s="75"/>
-      <c r="N33" s="75"/>
-      <c r="O33" s="75"/>
-      <c r="P33" s="75"/>
-      <c r="Q33" s="75"/>
-      <c r="R33" s="75"/>
-      <c r="S33" s="75"/>
-      <c r="T33" s="75"/>
-      <c r="U33" s="75"/>
-      <c r="V33" s="75"/>
-      <c r="W33" s="75"/>
-      <c r="X33" s="75"/>
+      <c r="N32" s="15"/>
+    </row>
+    <row r="35" spans="2:25">
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="75"/>
+      <c r="J35" s="75"/>
+      <c r="L35" s="75"/>
+      <c r="M35" s="75"/>
+      <c r="N35" s="75"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="75"/>
+      <c r="Q35" s="75"/>
+      <c r="R35" s="75"/>
+      <c r="S35" s="75"/>
+      <c r="T35" s="75"/>
+      <c r="U35" s="75"/>
+      <c r="V35" s="75"/>
+      <c r="W35" s="75"/>
+      <c r="X35" s="75"/>
+      <c r="Y35" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="17" t="str">
+        <f>'Iran Workbook'!G9</f>
+        <v>iYear</v>
+      </c>
+      <c r="B1" s="17" t="str">
+        <f>'Iran Workbook'!H9</f>
+        <v>iGDP</v>
+      </c>
+      <c r="C1" s="17" t="str">
+        <f>'Iran Workbook'!I9</f>
+        <v>iLabor</v>
+      </c>
+      <c r="D1" s="17" t="str">
+        <f>'Iran Workbook'!J9</f>
+        <v>iCapStk</v>
+      </c>
+      <c r="E1" s="17" t="str">
+        <f>'Iran Workbook'!K9</f>
+        <v>iQ</v>
+      </c>
+      <c r="F1" s="17" t="str">
+        <f>'Iran Workbook'!L9</f>
+        <v>iX</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="94">
+        <f>'Iran Workbook'!G12</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="95">
+        <f>'Iran Workbook'!H12</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="95">
+        <f>'Iran Workbook'!I12</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="95">
+        <f>'Iran Workbook'!J12</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="95">
+        <f>'Iran Workbook'!K12</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="95">
+        <f>'Iran Workbook'!L12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="94">
+        <f>'Iran Workbook'!G13</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="95">
+        <f>'Iran Workbook'!H13</f>
+        <v>1.0425075890787252</v>
+      </c>
+      <c r="C3" s="95">
+        <f>'Iran Workbook'!I13</f>
+        <v>0.9923206837799815</v>
+      </c>
+      <c r="D3" s="95">
+        <f>'Iran Workbook'!J13</f>
+        <v>1.0286817340947478</v>
+      </c>
+      <c r="E3" s="95">
+        <f>'Iran Workbook'!K13</f>
+        <v>1.0354751704424248</v>
+      </c>
+      <c r="F3" s="95">
+        <f>'Iran Workbook'!L13</f>
+        <v>1.0357688087521719</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="94">
+        <f>'Iran Workbook'!G14</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="95">
+        <f>'Iran Workbook'!H14</f>
+        <v>1.0260784365185593</v>
+      </c>
+      <c r="C4" s="95">
+        <f>'Iran Workbook'!I14</f>
+        <v>1.0258154818585306</v>
+      </c>
+      <c r="D4" s="95">
+        <f>'Iran Workbook'!J14</f>
+        <v>1.0451808359473445</v>
+      </c>
+      <c r="E4" s="95">
+        <f>'Iran Workbook'!K14</f>
+        <v>1.0685785542910753</v>
+      </c>
+      <c r="F4" s="95">
+        <f>'Iran Workbook'!L14</f>
+        <v>1.0689180927469208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="94">
+        <f>'Iran Workbook'!G15</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="95">
+        <f>'Iran Workbook'!H15</f>
+        <v>1.0224829191052323</v>
+      </c>
+      <c r="C5" s="95">
+        <f>'Iran Workbook'!I15</f>
+        <v>1.0326056463787794</v>
+      </c>
+      <c r="D5" s="95">
+        <f>'Iran Workbook'!J15</f>
+        <v>1.0479449851202445</v>
+      </c>
+      <c r="E5" s="95">
+        <f>'Iran Workbook'!K15</f>
+        <v>1.1367876415670517</v>
+      </c>
+      <c r="F5" s="95">
+        <f>'Iran Workbook'!L15</f>
+        <v>1.1376856578004559</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="94">
+        <f>'Iran Workbook'!G16</f>
+        <v>4</v>
+      </c>
+      <c r="B6" s="95">
+        <f>'Iran Workbook'!H16</f>
+        <v>1.0496023935123218</v>
+      </c>
+      <c r="C6" s="95">
+        <f>'Iran Workbook'!I16</f>
+        <v>1.0676674469765692</v>
+      </c>
+      <c r="D6" s="95">
+        <f>'Iran Workbook'!J16</f>
+        <v>1.0470682860130298</v>
+      </c>
+      <c r="E6" s="95">
+        <f>'Iran Workbook'!K16</f>
+        <v>1.1794323382104563</v>
+      </c>
+      <c r="F6" s="95">
+        <f>'Iran Workbook'!L16</f>
+        <v>1.1797195866624628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="94">
+        <f>'Iran Workbook'!G17</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="95">
+        <f>'Iran Workbook'!H17</f>
+        <v>1.1241372070440647</v>
+      </c>
+      <c r="C7" s="95">
+        <f>'Iran Workbook'!I17</f>
+        <v>1.0762276410999878</v>
+      </c>
+      <c r="D7" s="95">
+        <f>'Iran Workbook'!J17</f>
+        <v>1.0643931472693637</v>
+      </c>
+      <c r="E7" s="95">
+        <f>'Iran Workbook'!K17</f>
+        <v>1.2217207287451377</v>
+      </c>
+      <c r="F7" s="95">
+        <f>'Iran Workbook'!L17</f>
+        <v>1.2213614449700736</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="94">
+        <f>'Iran Workbook'!G18</f>
+        <v>6</v>
+      </c>
+      <c r="B8" s="95">
+        <f>'Iran Workbook'!H18</f>
+        <v>1.1621832051719463</v>
+      </c>
+      <c r="C8" s="95">
+        <f>'Iran Workbook'!I18</f>
+        <v>1.1451203214814862</v>
+      </c>
+      <c r="D8" s="95">
+        <f>'Iran Workbook'!J18</f>
+        <v>1.09182283707338</v>
+      </c>
+      <c r="E8" s="95">
+        <f>'Iran Workbook'!K18</f>
+        <v>1.3647844973964818</v>
+      </c>
+      <c r="F8" s="95">
+        <f>'Iran Workbook'!L18</f>
+        <v>1.3650633285601241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="94">
+        <f>'Iran Workbook'!G19</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="95">
+        <f>'Iran Workbook'!H19</f>
+        <v>1.1940354652739504</v>
+      </c>
+      <c r="C9" s="95">
+        <f>'Iran Workbook'!I19</f>
+        <v>1.2057762614790537</v>
+      </c>
+      <c r="D9" s="95">
+        <f>'Iran Workbook'!J19</f>
+        <v>1.1206413040564089</v>
+      </c>
+      <c r="E9" s="95">
+        <f>'Iran Workbook'!K19</f>
+        <v>1.4153780447913518</v>
+      </c>
+      <c r="F9" s="95">
+        <f>'Iran Workbook'!L19</f>
+        <v>1.4144342250706479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="94">
+        <f>'Iran Workbook'!G20</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="95">
+        <f>'Iran Workbook'!H20</f>
+        <v>1.2171307596077299</v>
+      </c>
+      <c r="C10" s="95">
+        <f>'Iran Workbook'!I20</f>
+        <v>1.2474506450804785</v>
+      </c>
+      <c r="D10" s="95">
+        <f>'Iran Workbook'!J20</f>
+        <v>1.1535537145767982</v>
+      </c>
+      <c r="E10" s="95">
+        <f>'Iran Workbook'!K20</f>
+        <v>1.4927197656780942</v>
+      </c>
+      <c r="F10" s="95">
+        <f>'Iran Workbook'!L20</f>
+        <v>1.4908857723563396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="94">
+        <f>'Iran Workbook'!G21</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="95">
+        <f>'Iran Workbook'!H21</f>
+        <v>1.2797242561828028</v>
+      </c>
+      <c r="C11" s="95">
+        <f>'Iran Workbook'!I21</f>
+        <v>1.3427875426021263</v>
+      </c>
+      <c r="D11" s="95">
+        <f>'Iran Workbook'!J21</f>
+        <v>1.1887396444944904</v>
+      </c>
+      <c r="E11" s="95">
+        <f>'Iran Workbook'!K21</f>
+        <v>1.5539588955476646</v>
+      </c>
+      <c r="F11" s="95">
+        <f>'Iran Workbook'!L21</f>
+        <v>1.5510817341155141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="94">
+        <f>'Iran Workbook'!G22</f>
+        <v>10</v>
+      </c>
+      <c r="B12" s="95">
+        <f>'Iran Workbook'!H22</f>
+        <v>1.3266846879948211</v>
+      </c>
+      <c r="C12" s="95">
+        <f>'Iran Workbook'!I22</f>
+        <v>1.4046771040381612</v>
+      </c>
+      <c r="D12" s="95">
+        <f>'Iran Workbook'!J22</f>
+        <v>1.2378857342019893</v>
+      </c>
+      <c r="E12" s="95">
+        <f>'Iran Workbook'!K22</f>
+        <v>1.6620445440994238</v>
+      </c>
+      <c r="F12" s="95">
+        <f>'Iran Workbook'!L22</f>
+        <v>1.6583023297085866</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="94">
+        <f>'Iran Workbook'!G23</f>
+        <v>11</v>
+      </c>
+      <c r="B13" s="95">
+        <f>'Iran Workbook'!H23</f>
+        <v>1.4263968716374038</v>
+      </c>
+      <c r="C13" s="95">
+        <f>'Iran Workbook'!I23</f>
+        <v>1.4662256242124556</v>
+      </c>
+      <c r="D13" s="95">
+        <f>'Iran Workbook'!J23</f>
+        <v>1.2994879219282018</v>
+      </c>
+      <c r="E13" s="95">
+        <f>'Iran Workbook'!K23</f>
+        <v>1.8149245739499966</v>
+      </c>
+      <c r="F13" s="95">
+        <f>'Iran Workbook'!L23</f>
+        <v>1.8108274724325999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="94">
+        <f>'Iran Workbook'!G24</f>
+        <v>12</v>
+      </c>
+      <c r="B14" s="95">
+        <f>'Iran Workbook'!H24</f>
+        <v>1.5278761952252229</v>
+      </c>
+      <c r="C14" s="95">
+        <f>'Iran Workbook'!I24</f>
+        <v>1.5669527354415114</v>
+      </c>
+      <c r="D14" s="95">
+        <f>'Iran Workbook'!J24</f>
+        <v>1.3727713879728678</v>
+      </c>
+      <c r="E14" s="95">
+        <f>'Iran Workbook'!K24</f>
+        <v>1.9103878204968034</v>
+      </c>
+      <c r="F14" s="95">
+        <f>'Iran Workbook'!L24</f>
+        <v>1.9053926591768511</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="94">
+        <f>'Iran Workbook'!G25</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="95">
+        <f>'Iran Workbook'!H25</f>
+        <v>1.6055603670752083</v>
+      </c>
+      <c r="C15" s="95">
+        <f>'Iran Workbook'!I25</f>
+        <v>1.7123166508885288</v>
+      </c>
+      <c r="D15" s="95">
+        <f>'Iran Workbook'!J25</f>
+        <v>1.4523552910265691</v>
+      </c>
+      <c r="E15" s="95">
+        <f>'Iran Workbook'!K25</f>
+        <v>1.9855840715413844</v>
+      </c>
+      <c r="F15" s="95">
+        <f>'Iran Workbook'!L25</f>
+        <v>1.978986980947947</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="94">
+        <f>'Iran Workbook'!G26</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="95">
+        <f>'Iran Workbook'!H26</f>
+        <v>1.6797889929926777</v>
+      </c>
+      <c r="C16" s="95">
+        <f>'Iran Workbook'!I26</f>
+        <v>1.7569037569931252</v>
+      </c>
+      <c r="D16" s="95">
+        <f>'Iran Workbook'!J26</f>
+        <v>1.5352797662135713</v>
+      </c>
+      <c r="E16" s="95">
+        <f>'Iran Workbook'!K26</f>
+        <v>2.264872229313418</v>
+      </c>
+      <c r="F16" s="95">
+        <f>'Iran Workbook'!L26</f>
+        <v>2.2580242095110754</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="94">
+        <f>'Iran Workbook'!G27</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="95">
+        <f>'Iran Workbook'!H27</f>
+        <v>1.7787925710136561</v>
+      </c>
+      <c r="C17" s="95">
+        <f>'Iran Workbook'!I27</f>
+        <v>1.7594397758824338</v>
+      </c>
+      <c r="D17" s="95">
+        <f>'Iran Workbook'!J27</f>
+        <v>1.618542052065739</v>
+      </c>
+      <c r="E17" s="95">
+        <f>'Iran Workbook'!K27</f>
+        <v>2.3667027015633595</v>
+      </c>
+      <c r="F17" s="95">
+        <f>'Iran Workbook'!L27</f>
+        <v>2.3611229336631401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="94">
+        <f>'Iran Workbook'!G28</f>
+        <v>16</v>
+      </c>
+      <c r="B18" s="95">
+        <f>'Iran Workbook'!H28</f>
+        <v>1.9179767122448801</v>
+      </c>
+      <c r="C18" s="95">
+        <f>'Iran Workbook'!I28</f>
+        <v>1.8044561053690826</v>
+      </c>
+      <c r="D18" s="95">
+        <f>'Iran Workbook'!J28</f>
+        <v>1.7074130673744605</v>
+      </c>
+      <c r="E18" s="95">
+        <f>'Iran Workbook'!K28</f>
+        <v>2.42511195449213</v>
+      </c>
+      <c r="F18" s="95">
+        <f>'Iran Workbook'!L28</f>
+        <v>2.4189262128003968</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="94">
+        <f>'Iran Workbook'!G29</f>
+        <v>17</v>
+      </c>
+      <c r="B19" s="95">
+        <f>'Iran Workbook'!H29</f>
+        <v>1.9620939733529292</v>
+      </c>
+      <c r="C19" s="95">
+        <f>'Iran Workbook'!I29</f>
+        <v>1.7369485759342249</v>
+      </c>
+      <c r="D19" s="95">
+        <f>'Iran Workbook'!J29</f>
+        <v>1.8001715863696077</v>
+      </c>
+      <c r="E19" s="95">
+        <f>'Iran Workbook'!K29</f>
+        <v>2.498205764678846</v>
+      </c>
+      <c r="F19" s="95">
+        <f>'Iran Workbook'!L29</f>
+        <v>2.4960181914910886</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="94">
+        <f>'Iran Workbook'!G30</f>
+        <v>18</v>
+      </c>
+      <c r="B20" s="95">
+        <f>'Iran Workbook'!H30</f>
+        <v>1.9974105276050005</v>
+      </c>
+      <c r="C20" s="95">
+        <f>'Iran Workbook'!I30</f>
+        <v>1.7804433072068904</v>
+      </c>
+      <c r="D20" s="95">
+        <f>'Iran Workbook'!J30</f>
+        <v>1.8938657872865223</v>
+      </c>
+      <c r="E20" s="95">
+        <f>'Iran Workbook'!K30</f>
+        <v>2.7790345832709171</v>
+      </c>
+      <c r="F20" s="95">
+        <f>'Iran Workbook'!L30</f>
+        <v>2.7762888939252521</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="94">
+        <f>'Iran Workbook'!G31</f>
+        <v>19</v>
+      </c>
+      <c r="B21" s="95">
+        <f>'Iran Workbook'!H31</f>
+        <v>2.055533685011679</v>
+      </c>
+      <c r="C21" s="95">
+        <f>'Iran Workbook'!I31</f>
+        <v>1.8469810667781668</v>
+      </c>
+      <c r="D21" s="95">
+        <f>'Iran Workbook'!J31</f>
+        <v>1.9875921606477385</v>
+      </c>
+      <c r="E21" s="95">
+        <f>'Iran Workbook'!K31</f>
+        <v>2.6340241858394191</v>
+      </c>
+      <c r="F21" s="95">
+        <f>'Iran Workbook'!L31</f>
+        <v>2.6237846706204704</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="94">
+        <f>'Iran Workbook'!G32</f>
+        <v>20</v>
+      </c>
+      <c r="B22" s="95">
+        <f>'Iran Workbook'!H32</f>
+        <v>2.097105214812482</v>
+      </c>
+      <c r="C22" s="95">
+        <f>'Iran Workbook'!I32</f>
+        <v>1.8675789761098966</v>
+      </c>
+      <c r="D22" s="95">
+        <f>'Iran Workbook'!J32</f>
+        <v>2.0860746936915198</v>
+      </c>
+      <c r="E22" s="95">
+        <f>'Iran Workbook'!K32</f>
+        <v>3.0448529057910276</v>
+      </c>
+      <c r="F22" s="95">
+        <f>'Iran Workbook'!L32</f>
+        <v>3.044836080007213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA27"/>
   <sheetViews>
@@ -5766,17 +6605,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="15" customFormat="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="79" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="15" customFormat="1">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="79" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:53">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="79" t="s">
         <v>98</v>
       </c>
     </row>
@@ -5837,19 +6676,19 @@
     </row>
     <row r="5" spans="1:53">
       <c r="A5" s="6"/>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="83" t="s">
+      <c r="E5" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="83" t="s">
+      <c r="F5" s="82" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5857,11 +6696,11 @@
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
     </row>
     <row r="7" spans="1:53">
       <c r="A7" s="6">
@@ -6337,7 +7176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG70"/>
   <sheetViews>
@@ -6660,140 +7499,140 @@
       </c>
     </row>
     <row r="28" spans="1:33" ht="15" customHeight="1">
-      <c r="A28" s="86" t="s">
+      <c r="A28" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="88" t="s">
+      <c r="B28" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="90" t="s">
+      <c r="C28" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="88" t="s">
+      <c r="D28" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="88" t="s">
+      <c r="E28" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="88" t="s">
+      <c r="F28" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="88" t="s">
+      <c r="G28" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="88" t="s">
+      <c r="H28" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="I28" s="88" t="s">
+      <c r="I28" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="J28" s="88" t="s">
+      <c r="J28" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="K28" s="88" t="s">
+      <c r="K28" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="L28" s="86" t="s">
+      <c r="L28" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="M28" s="90" t="s">
+      <c r="M28" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="N28" s="88" t="s">
+      <c r="N28" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="O28" s="88" t="s">
+      <c r="O28" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="P28" s="86" t="s">
+      <c r="P28" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="Q28" s="90" t="s">
+      <c r="Q28" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="R28" s="88" t="s">
+      <c r="R28" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="S28" s="88" t="s">
+      <c r="S28" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="T28" s="88" t="s">
+      <c r="T28" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="U28" s="88" t="s">
+      <c r="U28" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="V28" s="88" t="s">
+      <c r="V28" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="W28" s="88" t="s">
+      <c r="W28" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="X28" s="92" t="s">
+      <c r="X28" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="Y28" s="86" t="s">
+      <c r="Y28" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="Z28" s="90" t="s">
+      <c r="Z28" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="AA28" s="88" t="s">
+      <c r="AA28" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="AB28" s="88" t="s">
+      <c r="AB28" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="AC28" s="88" t="s">
+      <c r="AC28" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="AD28" s="88" t="s">
+      <c r="AD28" s="85" t="s">
         <v>87</v>
       </c>
-      <c r="AE28" s="88" t="s">
+      <c r="AE28" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="AF28" s="88" t="s">
+      <c r="AF28" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="AG28" s="92" t="s">
+      <c r="AG28" s="87" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="A29" s="87"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="91"/>
-      <c r="N29" s="89"/>
-      <c r="O29" s="89"/>
-      <c r="P29" s="87"/>
-      <c r="Q29" s="91"/>
-      <c r="R29" s="89"/>
-      <c r="S29" s="89"/>
-      <c r="T29" s="89"/>
-      <c r="U29" s="89"/>
-      <c r="V29" s="89"/>
-      <c r="W29" s="89"/>
-      <c r="X29" s="93"/>
-      <c r="Y29" s="87"/>
-      <c r="Z29" s="91"/>
-      <c r="AA29" s="89"/>
-      <c r="AB29" s="89"/>
-      <c r="AC29" s="89"/>
-      <c r="AD29" s="89"/>
-      <c r="AE29" s="89"/>
-      <c r="AF29" s="89"/>
-      <c r="AG29" s="93"/>
+      <c r="A29" s="92"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="86"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="92"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="86"/>
+      <c r="P29" s="92"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="86"/>
+      <c r="S29" s="86"/>
+      <c r="T29" s="86"/>
+      <c r="U29" s="86"/>
+      <c r="V29" s="86"/>
+      <c r="W29" s="86"/>
+      <c r="X29" s="88"/>
+      <c r="Y29" s="92"/>
+      <c r="Z29" s="90"/>
+      <c r="AA29" s="86"/>
+      <c r="AB29" s="86"/>
+      <c r="AC29" s="86"/>
+      <c r="AD29" s="86"/>
+      <c r="AE29" s="86"/>
+      <c r="AF29" s="86"/>
+      <c r="AG29" s="88"/>
     </row>
     <row r="30" spans="1:33">
       <c r="A30" s="45">
@@ -9577,19 +10416,16 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AE28:AE29"/>
-    <mergeCell ref="AF28:AF29"/>
-    <mergeCell ref="AG28:AG29"/>
-    <mergeCell ref="Z28:Z29"/>
-    <mergeCell ref="AA28:AA29"/>
-    <mergeCell ref="AB28:AB29"/>
-    <mergeCell ref="AC28:AC29"/>
-    <mergeCell ref="AD28:AD29"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="V28:V29"/>
-    <mergeCell ref="W28:W29"/>
-    <mergeCell ref="X28:X29"/>
-    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
     <mergeCell ref="K28:K29"/>
     <mergeCell ref="T28:T29"/>
     <mergeCell ref="L28:L29"/>
@@ -9600,16 +10436,19 @@
     <mergeCell ref="Q28:Q29"/>
     <mergeCell ref="R28:R29"/>
     <mergeCell ref="S28:S29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="V28:V29"/>
+    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="X28:X29"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="AF28:AF29"/>
+    <mergeCell ref="AG28:AG29"/>
+    <mergeCell ref="Z28:Z29"/>
+    <mergeCell ref="AA28:AA29"/>
+    <mergeCell ref="AB28:AB29"/>
+    <mergeCell ref="AC28:AC29"/>
+    <mergeCell ref="AD28:AD29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>